<commit_message>
Caricamento del file csv + punto A ed E
1) Modificata la generazione dei dati nel file crea_dataset
2) Creazione del codice c# per il caricamento e due punti
</commit_message>
<xml_diff>
--- a/Matematica/dati.xlsx
+++ b/Matematica/dati.xlsx
@@ -357,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1637,6 +1637,104 @@
         <v>48877</v>
       </c>
     </row>
+    <row r="92" spans="1:4">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>183957</v>
+      </c>
+      <c r="C92">
+        <v>24648</v>
+      </c>
+      <c r="D92">
+        <v>51600</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>187327</v>
+      </c>
+      <c r="C93">
+        <v>25085</v>
+      </c>
+      <c r="D93">
+        <v>54543</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>189973</v>
+      </c>
+      <c r="C94">
+        <v>25549</v>
+      </c>
+      <c r="D94">
+        <v>57576</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>192994</v>
+      </c>
+      <c r="C95">
+        <v>25969</v>
+      </c>
+      <c r="D95">
+        <v>60498</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>195351</v>
+      </c>
+      <c r="C96">
+        <v>26384</v>
+      </c>
+      <c r="D96">
+        <v>63120</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>197675</v>
+      </c>
+      <c r="C97">
+        <v>26644</v>
+      </c>
+      <c r="D97">
+        <v>64928</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>199414</v>
+      </c>
+      <c r="C98">
+        <v>26977</v>
+      </c>
+      <c r="D98">
+        <v>66624</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiunta tessera sanitaria + mirror fix
</commit_message>
<xml_diff>
--- a/Matematica/dati.xlsx
+++ b/Matematica/dati.xlsx
@@ -357,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1735,6 +1735,202 @@
         <v>66624</v>
       </c>
     </row>
+    <row r="99" spans="1:4">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>201505</v>
+      </c>
+      <c r="C99">
+        <v>27359</v>
+      </c>
+      <c r="D99">
+        <v>68941</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>203591</v>
+      </c>
+      <c r="C100">
+        <v>27682</v>
+      </c>
+      <c r="D100">
+        <v>71252</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>205463</v>
+      </c>
+      <c r="C101">
+        <v>27967</v>
+      </c>
+      <c r="D101">
+        <v>75945</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>207428</v>
+      </c>
+      <c r="C102">
+        <v>28236</v>
+      </c>
+      <c r="D102">
+        <v>78249</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>209328</v>
+      </c>
+      <c r="C103">
+        <v>28710</v>
+      </c>
+      <c r="D103">
+        <v>79914</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>210717</v>
+      </c>
+      <c r="C104">
+        <v>28884</v>
+      </c>
+      <c r="D104">
+        <v>81654</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>211938</v>
+      </c>
+      <c r="C105">
+        <v>29079</v>
+      </c>
+      <c r="D105">
+        <v>82879</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>213013</v>
+      </c>
+      <c r="C106">
+        <v>29315</v>
+      </c>
+      <c r="D106">
+        <v>85231</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <v>214457</v>
+      </c>
+      <c r="C107">
+        <v>29684</v>
+      </c>
+      <c r="D107">
+        <v>93245</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <v>215858</v>
+      </c>
+      <c r="C108">
+        <v>29958</v>
+      </c>
+      <c r="D108">
+        <v>96276</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <v>217185</v>
+      </c>
+      <c r="C109">
+        <v>30201</v>
+      </c>
+      <c r="D109">
+        <v>99023</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>218268</v>
+      </c>
+      <c r="C110">
+        <v>30395</v>
+      </c>
+      <c r="D110">
+        <v>103031</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>219070</v>
+      </c>
+      <c r="C111">
+        <v>30560</v>
+      </c>
+      <c r="D111">
+        <v>105186</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <v>219814</v>
+      </c>
+      <c r="C112">
+        <v>30739</v>
+      </c>
+      <c r="D112">
+        <v>106587</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>